<commit_message>
Make critical error happen earlier
</commit_message>
<xml_diff>
--- a/DiagnosticsInputsFaultsAfterTimePeriod.xlsx
+++ b/DiagnosticsInputsFaultsAfterTimePeriod.xlsx
@@ -250,12 +250,12 @@
   <dimension ref="A1:H1463"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A293" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A257" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C302" activeCellId="0" sqref="C302:D302"/>
+      <selection pane="bottomLeft" activeCell="B270" activeCellId="0" sqref="B270"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="9.66"/>
@@ -7234,7 +7234,7 @@
         <v>4.005</v>
       </c>
       <c r="B269" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C269" s="3" t="n">
         <v>0</v>
@@ -10692,7 +10692,7 @@
         <v>6</v>
       </c>
       <c r="B402" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C402" s="3" t="n">
         <v>1</v>

</xml_diff>